<commit_message>
Commiting changes with the Extent Report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/actidata.xlsx
+++ b/src/test/resources/testdata/actidata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MuthuMalai\git\com.qa.actitime\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A7C723-FB17-403B-A9B0-085BEAF42DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B3ABC2-134A-4653-8052-B7D1BFDB9080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>admin</t>
   </si>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,22 +390,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>